<commit_message>
from avro to RDD
</commit_message>
<xml_diff>
--- a/P2/development/columns _to_be_prepared.xlsx
+++ b/P2/development/columns _to_be_prepared.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pietro/Desktop/BDM/Project/DataImporta/P2/development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D65DED4-86ED-D24F-966A-88DCD1E53B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2763EA-9F0E-2B4E-B562-72595C6AFFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{F76398F3-3CAD-4CD7-B760-50FC475CC7DB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F76398F3-3CAD-4CD7-B760-50FC475CC7DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="129">
   <si>
     <t xml:space="preserve">Descripcion de la Partida Aduanera </t>
   </si>
@@ -370,12 +370,75 @@
   <si>
     <t>CO_VIA(metadata VIA)</t>
   </si>
+  <si>
+    <t>CHILE (columns names to be exported from the metadata)</t>
+  </si>
+  <si>
+    <t>ADU</t>
+  </si>
+  <si>
+    <t>NUMEROCRIPTADO?</t>
+  </si>
+  <si>
+    <t>CODPAISCON</t>
+  </si>
+  <si>
+    <t>PA_ORIG</t>
+  </si>
+  <si>
+    <t>VIA_TRAN</t>
+  </si>
+  <si>
+    <t>PTO_EMB</t>
+  </si>
+  <si>
+    <t>Puerto de Desembarque</t>
+  </si>
+  <si>
+    <t>PTO_DESEM</t>
+  </si>
+  <si>
+    <t>FLETE</t>
+  </si>
+  <si>
+    <t>BCO_COM</t>
+  </si>
+  <si>
+    <t>SEGURO</t>
+  </si>
+  <si>
+    <t>TOT_PESO</t>
+  </si>
+  <si>
+    <t>TOT_ITEMS</t>
+  </si>
+  <si>
+    <t>DNOMBRE + DMARCA + DVARIEDAD + DOTRO1 + DOTRO2 + ATR_5 +  ATR_6</t>
+  </si>
+  <si>
+    <t>PRE_UNIT</t>
+  </si>
+  <si>
+    <t>CODCOMRS</t>
+  </si>
+  <si>
+    <t>FECVENCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FOB</t>
+  </si>
+  <si>
+    <t>FOB + FLETE</t>
+  </si>
+  <si>
+    <t>FOB + FLETE + SEGURO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,8 +467,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,8 +488,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -442,30 +524,31 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -780,489 +863,545 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD43CE0-143E-4F48-81C1-05D42DC8D3CA}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F2:F21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="68.83203125" customWidth="1"/>
-    <col min="5" max="5" width="190.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.1640625" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="5"/>
+      <c r="E2" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="9" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="10" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="5" t="s">
         <v>70</v>
       </c>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="9" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="10" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="5" t="s">
         <v>59</v>
       </c>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="5" t="s">
         <v>63</v>
       </c>
       <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="5" t="s">
         <v>65</v>
       </c>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="5" t="s">
         <v>66</v>
       </c>
       <c r="D36" s="5"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="5" t="s">
         <v>67</v>
       </c>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="5" t="s">
         <v>68</v>
       </c>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="5" t="s">
         <v>69</v>
       </c>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+    <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
         <v>99</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>94</v>
       </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D44" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>